<commit_message>
adding Gerosa et al. example
</commit_message>
<xml_diff>
--- a/examples/metabolic_kinetics/template.xlsx
+++ b/examples/metabolic_kinetics/template.xlsx
@@ -16,10 +16,10 @@
     <sheet name="!!Regulations" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!!_Schema'!$A$2:$G$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!!_Schema'!$A$2:$G$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$3:$C$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'!!Compartments'!$A$2:$B$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'!!Metabolites'!$A$2:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'!!Metabolites'!$A$2:$C$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'!!Reactions'!$A$2:$M$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'!!References'!$A$2:$I$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'!!Regulations'!$A$2:$D$2</definedName>
@@ -103,20 +103,6 @@
       </text>
     </comment>
     <comment ref="C2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -518,7 +504,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="149">
   <si>
     <t>'!!_Schema'!A1</t>
   </si>
@@ -538,10 +524,10 @@
     <t>'!!Regulations'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables objTablesVersion='1.0.0' date='2020-05-29 00:17:39'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-05-29 00:17:39' objTablesVersion='1.0.0'</t>
+    <t>!!!ObjTables objTablesVersion='1.0.0' date='2020-06-02 16:10:23'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-06-02 16:10:23' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -574,7 +560,7 @@
     <t>Regulations</t>
   </si>
   <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-05-29 00:17:39' objTablesVersion='1.0.0'</t>
+    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-06-02 16:10:23' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -637,48 +623,48 @@
     <t>Formula</t>
   </si>
   <si>
+    <t>Reaction</t>
+  </si>
+  <si>
+    <t>coupled_to_biomass</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Coupled to biomass</t>
+  </si>
+  <si>
+    <t>ec_number</t>
+  </si>
+  <si>
+    <t>Regex(r'\d+\.\d+\.\d+\.\d+', none=True, default=None, default_cleaned_value=None)</t>
+  </si>
+  <si>
+    <t>EC number</t>
+  </si>
+  <si>
+    <t>equation</t>
+  </si>
+  <si>
+    <t>chem.ReactionEquation</t>
+  </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <t>gene_rule</t>
+  </si>
+  <si>
+    <t>Gene rule</t>
+  </si>
+  <si>
     <t>id_i_a_f1260</t>
   </si>
   <si>
     <t>Id (iAF1260 [Ref1])</t>
   </si>
   <si>
-    <t>Reaction</t>
-  </si>
-  <si>
-    <t>coupled_to_biomass</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Coupled to biomass</t>
-  </si>
-  <si>
-    <t>ec_number</t>
-  </si>
-  <si>
-    <t>Regex(r'\d+\.\d+\.\d+\.\d+', none=True, default=None, default_cleaned_value=None)</t>
-  </si>
-  <si>
-    <t>EC number</t>
-  </si>
-  <si>
-    <t>equation</t>
-  </si>
-  <si>
-    <t>chem.ReactionEquation</t>
-  </si>
-  <si>
-    <t>Equation</t>
-  </si>
-  <si>
-    <t>gene_rule</t>
-  </si>
-  <si>
-    <t>Gene rule</t>
-  </si>
-  <si>
     <t>k_cat_k_ms</t>
   </si>
   <si>
@@ -877,24 +863,24 @@
     <t>Value</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Compartment' name='Compartments' date='2020-05-29 00:17:39' objTablesVersion='1.0.0'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Compartment' name='Compartments' date='2020-06-02 16:10:23' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Id</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Metabolite' name='Metabolites' date='2020-05-29 00:17:39' objTablesVersion='1.0.0'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Metabolite' name='Metabolites' date='2020-06-02 16:10:23' objTablesVersion='1.0.0'</t>
+  </si>
+  <si>
+    <t>!Formula</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Reaction' name='Reactions' date='2020-06-02 16:10:23' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Id (iAF1260 [Ref1])</t>
   </si>
   <si>
-    <t>!Formula</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Reaction' name='Reactions' date='2020-05-29 00:17:39' objTablesVersion='1.0.0'</t>
-  </si>
-  <si>
     <t>!Equation</t>
   </si>
   <si>
@@ -925,7 +911,7 @@
     <t>!Coupled to biomass</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Reference' name='References' date='2020-05-29 00:17:39' objTablesVersion='1.0.0'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Reference' name='References' date='2020-06-02 16:10:23' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Title</t>
@@ -952,7 +938,7 @@
     <t>!PubMed id</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Regulation' name='Regulations' date='2020-05-29 00:17:39' objTablesVersion='1.0.0'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Regulation' name='Regulations' date='2020-06-02 16:10:23' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Reaction</t>
@@ -1447,7 +1433,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1610,7 +1596,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.01" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -1622,99 +1608,99 @@
         <v>33</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="15.01" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="15.01" customHeight="1">
       <c r="A11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="15.01" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15.01" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="15.01" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>50</v>
@@ -1724,216 +1710,216 @@
     </row>
     <row r="15" spans="1:7" ht="15.01" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="15.01" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15.01" customHeight="1">
       <c r="A17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15.01" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="15.01" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" ht="15.01" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="15.01" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="15.01" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="E22" s="4" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" ht="15.01" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="15.01" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="15.01" customHeight="1">
       <c r="A25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="15.01" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>29</v>
@@ -1942,17 +1928,17 @@
         <v>69</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="15.01" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>29</v>
@@ -1961,17 +1947,17 @@
         <v>69</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="15.01" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>29</v>
@@ -1980,17 +1966,17 @@
         <v>69</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="15.01" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>29</v>
@@ -1999,17 +1985,17 @@
         <v>69</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" ht="15.01" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>29</v>
@@ -2018,17 +2004,17 @@
         <v>69</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="15.01" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>29</v>
@@ -2040,14 +2026,14 @@
         <v>74</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="15.01" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>29</v>
@@ -2056,17 +2042,17 @@
         <v>69</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" ht="15.01" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>29</v>
@@ -2075,55 +2061,55 @@
         <v>69</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="15.01" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F34" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="15.01" customHeight="1">
       <c r="A35" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="15.01" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>29</v>
@@ -2132,17 +2118,17 @@
         <v>88</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="15.01" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>29</v>
@@ -2151,17 +2137,17 @@
         <v>88</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="15.01" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>29</v>
@@ -2170,55 +2156,55 @@
         <v>88</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="15.01" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>88</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F39" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" ht="15.01" customHeight="1">
       <c r="A40" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>100</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" ht="15.01" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>29</v>
@@ -2227,17 +2213,17 @@
         <v>100</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" ht="15.01" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>29</v>
@@ -2246,17 +2232,17 @@
         <v>100</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" ht="15.01" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>29</v>
@@ -2268,14 +2254,14 @@
         <v>33</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" ht="15.01" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>29</v>
@@ -2284,17 +2270,17 @@
         <v>100</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" ht="15.01" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>29</v>
@@ -2306,14 +2292,14 @@
         <v>112</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" ht="15.01" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>29</v>
@@ -2322,42 +2308,23 @@
         <v>100</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A47" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
-  <autoFilter ref="A2:G47"/>
+  <autoFilter ref="A2:G46"/>
   <hyperlinks>
     <hyperlink ref="A3" location="'!!Compartments'!A1" tooltip="Click to view compartments" display="'!!Compartments'!A1"/>
     <hyperlink ref="A6" location="'!!Metabolites'!A1" tooltip="Click to view metabolites" display="'!!Metabolites'!A1"/>
-    <hyperlink ref="A11" location="'!!Reactions'!A1" tooltip="Click to view reactions" display="'!!Reactions'!A1"/>
-    <hyperlink ref="A25" location="'!!References'!A1" tooltip="Click to view references" display="'!!References'!A1"/>
-    <hyperlink ref="A35" location="'!!Regulations'!A1" tooltip="Click to view regulations" display="'!!Regulations'!A1"/>
+    <hyperlink ref="A10" location="'!!Reactions'!A1" tooltip="Click to view reactions" display="'!!Reactions'!A1"/>
+    <hyperlink ref="A24" location="'!!References'!A1" tooltip="Click to view references" display="'!!References'!A1"/>
+    <hyperlink ref="A34" location="'!!Regulations'!A1" tooltip="Click to view regulations" display="'!!Regulations'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2450,7 +2417,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -2459,106 +2426,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="16384" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.01" customHeight="1">
+    <row r="1" spans="1:3" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="2" spans="1:3" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="3" spans="1:3" ht="15.01" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="4" spans="1:3" ht="15.01" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="5" spans="1:3" ht="15.01" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="6" spans="1:3" ht="15.01" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="7" spans="1:3" ht="15.01" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="8" spans="1:3" ht="15.01" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="9" spans="1:3" ht="15.01" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="10" spans="1:3" ht="15.01" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="11" spans="1:3" ht="15.01" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.01" customHeight="1">
+    </row>
+    <row r="12" spans="1:3" ht="15.01" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
-  <autoFilter ref="A2:D2"/>
-  <dataValidations count="4">
+  <autoFilter ref="A2:C2"/>
+  <dataValidations count="3">
     <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A3:A12">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id (iAF1260 [Ref1])" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Id (iAF1260 [Ref1])" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B12">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B12">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="C3:C12">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Formula" error="Value must be an chemical formula (e.g. &quot;H2O&quot;)." promptTitle="Formula" prompt="Enter an chemical formula (e.g. &quot;H2O&quot;)." sqref="D3:D12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Formula" error="Value must be an chemical formula (e.g. &quot;H2O&quot;)." promptTitle="Formula" prompt="Enter an chemical formula (e.g. &quot;H2O&quot;)." sqref="C3:C12"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2582,7 +2532,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2602,7 +2552,7 @@
         <v>120</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>19</v>

</xml_diff>